<commit_message>
medio que ya esta todo solo falta corregir el 4to grafico
</commit_message>
<xml_diff>
--- a/Autoevaluación.xlsx
+++ b/Autoevaluación.xlsx
@@ -327,40 +327,44 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -651,310 +655,310 @@
   </sheetPr>
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="89.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="89.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="7" t="n">
+      <c r="C7" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+    </row>
+    <row r="8" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="8"/>
-    </row>
-    <row r="8" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="B8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+    </row>
+    <row r="9" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="9"/>
+    </row>
+    <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+      <c r="P10" s="9"/>
+    </row>
+    <row r="11" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="8" t="n">
+        <v>10</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+    </row>
+    <row r="12" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="8" t="n">
         <v>9</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="D12" s="8"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+    </row>
+    <row r="13" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="C8" s="7" t="n">
+      <c r="D13" s="8"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="9"/>
+    </row>
+    <row r="14" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-    </row>
-    <row r="9" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="7" t="n">
+      <c r="D14" s="8"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+    </row>
+    <row r="15" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-    </row>
-    <row r="10" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="7" t="n">
+      <c r="D15" s="8"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+    </row>
+    <row r="16" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-    </row>
-    <row r="11" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="7" t="n">
-        <v>8</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-    </row>
-    <row r="12" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="7" t="n">
-        <v>9</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-    </row>
-    <row r="13" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="7" t="n">
-        <v>10</v>
-      </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-    </row>
-    <row r="14" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="7" t="n">
-        <v>7</v>
-      </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-    </row>
-    <row r="15" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="7" t="n">
-        <v>9</v>
-      </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-    </row>
-    <row r="16" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="7" t="n">
-        <v>9</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>